<commit_message>
wip: add eda and test file
</commit_message>
<xml_diff>
--- a/data/Field Descriptions.xlsx
+++ b/data/Field Descriptions.xlsx
@@ -1,12 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView windowWidth="22368" windowHeight="9264"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -343,119 +346,710 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="24">
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="16.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16.0"/>
-      <color rgb="FF000000"/>
-      <name val="Century Gothic"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="16.0"/>
-      <color rgb="FF000000"/>
-      <name val="&quot;Century Gothic&quot;"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="16.0"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Century Gothic"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD6DCE4"/>
-        <bgColor rgb="FFD6DCE4"/>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
-    <border/>
+  <borders count="9">
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
+      <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top/>
-      <bottom/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF7F7F7F"/>
       </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFB2B2B2"/>
       </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -645,539 +1239,541 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B1017"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.2166666666667" defaultRowHeight="15" customHeight="1" outlineLevelCol="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="48.67"/>
-    <col customWidth="1" min="2" max="2" width="122.11"/>
-    <col customWidth="1" min="3" max="26" width="10.56"/>
+    <col min="1" max="1" width="48.6666666666667" customWidth="1"/>
+    <col min="2" max="2" width="122.108333333333" customWidth="1"/>
+    <col min="3" max="26" width="10.5583333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="1" customFormat="1" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="2" t="s">
+    <row r="3" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="5" t="s">
+    <row r="4" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="5" t="s">
+    <row r="5" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="5" t="s">
+    <row r="6" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="5" t="s">
+    <row r="7" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="5" t="s">
+    <row r="8" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="5" t="s">
+    <row r="9" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="7" t="s">
+    <row r="10" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="5" t="s">
+    <row r="11" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="5" t="s">
+    <row r="12" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="7" t="s">
+    <row r="13" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="7" t="s">
+    <row r="14" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="2" t="s">
+    <row r="15" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="7" t="s">
+    <row r="16" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="5" t="s">
+    <row r="17" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="5" t="s">
+    <row r="18" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="5" t="s">
+    <row r="19" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="5" t="s">
+    <row r="20" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="5" t="s">
+    <row r="21" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A21" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="5" t="s">
+    <row r="22" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A22" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="5" t="s">
+    <row r="23" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A23" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="5" t="s">
+    <row r="24" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A24" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="5" t="s">
+    <row r="25" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A25" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="5" t="s">
+    <row r="26" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A26" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="7" t="s">
+    <row r="27" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A27" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="7" t="s">
+    <row r="28" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A28" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="7" t="s">
+    <row r="29" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A29" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="7" t="s">
+    <row r="30" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A30" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="2" t="s">
+    <row r="31" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A31" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="7" t="s">
+    <row r="32" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A32" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="5" t="s">
+    <row r="33" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A33" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="5" t="s">
+    <row r="34" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A34" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="5" t="s">
+    <row r="35" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A35" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="5" t="s">
+    <row r="36" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A36" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="5" t="s">
+    <row r="37" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A37" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="5" t="s">
+    <row r="38" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A38" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="5" t="s">
+    <row r="39" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A39" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="5" t="s">
+    <row r="40" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A40" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="5" t="s">
+    <row r="41" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A41" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="2" t="s">
+    <row r="42" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A42" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="2" t="s">
+    <row r="43" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A43" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="2" t="s">
+    <row r="44" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A44" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="2" t="s">
+    <row r="45" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A45" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="2" t="s">
+    <row r="46" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A46" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="2" t="s">
+    <row r="47" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A47" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="2" t="s">
+    <row r="48" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A48" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="2" t="s">
+    <row r="49" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A49" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="7" t="s">
+    <row r="50" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A50" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="7" t="s">
+    <row r="51" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A51" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="7" t="s">
+    <row r="52" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A52" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="7" t="s">
+    <row r="53" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A53" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="2" t="s">
+    <row r="54" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A54" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="2" t="s">
+    <row r="55" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A55" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="7" t="s">
+    <row r="56" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A56" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="7" t="s">
+    <row r="57" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A57" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="7"/>
-      <c r="B58" s="8"/>
-    </row>
-    <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="7"/>
-      <c r="B59" s="8"/>
-    </row>
-    <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="7"/>
-      <c r="B60" s="8"/>
-    </row>
-    <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="7"/>
-      <c r="B61" s="8"/>
-    </row>
-    <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="7"/>
-      <c r="B62" s="8"/>
-    </row>
-    <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="7"/>
-      <c r="B63" s="8"/>
-    </row>
-    <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="7"/>
-      <c r="B64" s="8"/>
-    </row>
-    <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="7"/>
-      <c r="B65" s="8"/>
-    </row>
-    <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="7"/>
-      <c r="B66" s="8"/>
-    </row>
-    <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="7"/>
-      <c r="B67" s="8"/>
-    </row>
-    <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="7"/>
-      <c r="B68" s="8"/>
-    </row>
-    <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="7"/>
-      <c r="B69" s="8"/>
-    </row>
-    <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="7"/>
-      <c r="B70" s="8"/>
-    </row>
-    <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="7"/>
-      <c r="B71" s="8"/>
-    </row>
-    <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="7"/>
-      <c r="B72" s="8"/>
+    <row r="58" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+    </row>
+    <row r="59" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+    </row>
+    <row r="60" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+    </row>
+    <row r="61" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+    </row>
+    <row r="62" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+    </row>
+    <row r="63" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+    </row>
+    <row r="64" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+    </row>
+    <row r="65" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+    </row>
+    <row r="66" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+    </row>
+    <row r="67" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+    </row>
+    <row r="68" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+    </row>
+    <row r="69" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+    </row>
+    <row r="70" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+    </row>
+    <row r="71" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+    </row>
+    <row r="72" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
     </row>
     <row r="73" ht="15.75" customHeight="1"/>
     <row r="74" ht="15.75" customHeight="1"/>
@@ -2125,9 +2721,8 @@
     <row r="1016" ht="15.75" customHeight="1"/>
     <row r="1017" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="1" orientation="landscape"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>